<commit_message>
Added constructor adaptation strategies, store results for constructor calls, split adaptation into two parts
</commit_message>
<xml_diff>
--- a/backend/arena/calc3_adaptation.xlsx
+++ b/backend/arena/calc3_adaptation.xlsx
@@ -30,19 +30,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -78,7 +72,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -86,17 +80,11 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,11 +394,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -419,25 +407,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="3">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="1">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1"/>
@@ -445,10 +433,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>3</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Small improvements to adaptation
</commit_message>
<xml_diff>
--- a/backend/arena/calc3_adaptation.xlsx
+++ b/backend/arena/calc3_adaptation.xlsx
@@ -407,12 +407,8 @@
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="1">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1">
-        <v>3</v>
-      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1">

</xml_diff>